<commit_message>
add data folder to repository
</commit_message>
<xml_diff>
--- a/data/IUU.xlsx
+++ b/data/IUU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruna Miguel\illegal_fishing\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC205A6-5CF3-448C-A655-A52234A6F07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A7FF1AE-A1F3-4FD5-8A7B-7A582D7A456E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11805" yWindow="765" windowWidth="5520" windowHeight="10515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="154">
   <si>
     <t>Country</t>
   </si>
@@ -39,15 +39,9 @@
     <t>China</t>
   </si>
   <si>
-    <t>Taiwan</t>
-  </si>
-  <si>
     <t>Cambodia</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
     <t>Vietnam</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>India</t>
   </si>
   <si>
-    <t>Tanzania</t>
-  </si>
-  <si>
     <t>Japan</t>
   </si>
   <si>
@@ -126,9 +117,6 @@
     <t>Saint Lucia</t>
   </si>
   <si>
-    <t>Iran</t>
-  </si>
-  <si>
     <t>Haiti</t>
   </si>
   <si>
@@ -168,9 +156,6 @@
     <t>Angola</t>
   </si>
   <si>
-    <t>Venezuela</t>
-  </si>
-  <si>
     <t>Turkey</t>
   </si>
   <si>
@@ -186,9 +171,6 @@
     <t>Sri Lanka</t>
   </si>
   <si>
-    <t xml:space="preserve">Morocco </t>
-  </si>
-  <si>
     <t>Colombia</t>
   </si>
   <si>
@@ -240,9 +222,6 @@
     <t>Gambia</t>
   </si>
   <si>
-    <t xml:space="preserve">Dominica </t>
-  </si>
-  <si>
     <t>Maldives</t>
   </si>
   <si>
@@ -297,9 +276,6 @@
     <t>Kuwait</t>
   </si>
   <si>
-    <t xml:space="preserve">Greece </t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -318,12 +294,6 @@
     <t>Suriname</t>
   </si>
   <si>
-    <t>Marshall Island</t>
-  </si>
-  <si>
-    <t>Solomon Island</t>
-  </si>
-  <si>
     <t>Bahamas</t>
   </si>
   <si>
@@ -487,6 +457,39 @@
   </si>
   <si>
     <t>United States</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Iran, Islamic Republic of</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Taiwan, Province of China</t>
+  </si>
+  <si>
+    <t>Tanzania, United Republic of</t>
+  </si>
+  <si>
+    <t>Venezuela, Bolivarian Republic of</t>
   </si>
 </sst>
 </file>
@@ -804,10 +807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B152"/>
+  <dimension ref="A1:B153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -833,7 +836,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>151</v>
       </c>
       <c r="B3">
         <v>3.34</v>
@@ -841,7 +844,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>3.23</v>
@@ -849,7 +852,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>149</v>
       </c>
       <c r="B5">
         <v>3.16</v>
@@ -857,7 +860,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>3.16</v>
@@ -865,7 +868,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>3.01</v>
@@ -873,7 +876,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>2.96</v>
@@ -881,7 +884,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2.77</v>
@@ -889,7 +892,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>2.76</v>
@@ -897,7 +900,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>2.75</v>
@@ -905,7 +908,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>2.73</v>
@@ -913,7 +916,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>2.73</v>
@@ -921,7 +924,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>2.71</v>
@@ -929,7 +932,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2.71</v>
@@ -937,7 +940,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>2.7</v>
@@ -945,7 +948,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B17">
         <v>2.69</v>
@@ -953,7 +956,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18">
         <v>2.68</v>
@@ -961,7 +964,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>152</v>
       </c>
       <c r="B19">
         <v>2.65</v>
@@ -969,7 +972,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20">
         <v>2.63</v>
@@ -977,7 +980,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B21">
         <v>2.61</v>
@@ -985,7 +988,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>2.61</v>
@@ -993,7 +996,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B23">
         <v>2.61</v>
@@ -1001,7 +1004,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>2.6</v>
@@ -1009,7 +1012,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>2.58</v>
@@ -1017,7 +1020,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B26">
         <v>2.58</v>
@@ -1025,7 +1028,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B27">
         <v>2.57</v>
@@ -1033,7 +1036,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>2.56</v>
@@ -1041,7 +1044,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B29">
         <v>2.56</v>
@@ -1049,7 +1052,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>2.5499999999999998</v>
@@ -1057,7 +1060,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B31">
         <v>2.5299999999999998</v>
@@ -1065,7 +1068,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B32">
         <v>2.5299999999999998</v>
@@ -1073,7 +1076,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B33">
         <v>2.52</v>
@@ -1081,7 +1084,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B34">
         <v>2.5099999999999998</v>
@@ -1089,7 +1092,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B35">
         <v>2.5099999999999998</v>
@@ -1097,7 +1100,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="B36">
         <v>2.5</v>
@@ -1105,15 +1108,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B37">
-        <v>2.4900000000000002</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B38">
         <v>2.4900000000000002</v>
@@ -1121,39 +1124,39 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="B39">
-        <v>2.48</v>
+        <v>2.4900000000000002</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B40">
-        <v>2.4700000000000002</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B41">
-        <v>2.46</v>
+        <v>2.4700000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B42">
-        <v>2.4500000000000002</v>
+        <v>2.46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B43">
         <v>2.4500000000000002</v>
@@ -1161,47 +1164,47 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B44">
-        <v>2.44</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B45">
-        <v>2.4300000000000002</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>35</v>
       </c>
       <c r="B46">
-        <v>2.42</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>131</v>
       </c>
       <c r="B47">
-        <v>2.41</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B48">
-        <v>2.39</v>
+        <v>2.41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B49">
         <v>2.39</v>
@@ -1209,15 +1212,15 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B50">
-        <v>2.37</v>
+        <v>2.39</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B51">
         <v>2.37</v>
@@ -1225,7 +1228,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B52">
         <v>2.37</v>
@@ -1233,31 +1236,31 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B53">
-        <v>2.36</v>
+        <v>2.37</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>153</v>
       </c>
       <c r="B54">
-        <v>2.34</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B55">
-        <v>2.33</v>
+        <v>2.34</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B56">
         <v>2.33</v>
@@ -1265,7 +1268,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B57">
         <v>2.33</v>
@@ -1273,15 +1276,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B58">
-        <v>2.3199999999999998</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>148</v>
       </c>
       <c r="B59">
         <v>2.3199999999999998</v>
@@ -1289,15 +1292,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B60">
-        <v>2.31</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B61">
         <v>2.31</v>
@@ -1305,15 +1308,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>137</v>
+        <v>48</v>
       </c>
       <c r="B62">
-        <v>2.2999999999999998</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="B63">
         <v>2.2999999999999998</v>
@@ -1321,7 +1324,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B64">
         <v>2.2999999999999998</v>
@@ -1329,7 +1332,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B65">
         <v>2.2999999999999998</v>
@@ -1337,15 +1340,15 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="B66">
-        <v>2.29</v>
+        <v>2.2999999999999998</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>152</v>
+        <v>52</v>
       </c>
       <c r="B67">
         <v>2.29</v>
@@ -1353,23 +1356,23 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
       <c r="B68">
-        <v>2.2799999999999998</v>
+        <v>2.29</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B69">
-        <v>2.27</v>
+        <v>2.2799999999999998</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B70">
         <v>2.27</v>
@@ -1377,7 +1380,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B71">
         <v>2.27</v>
@@ -1385,15 +1388,15 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B72">
-        <v>2.2599999999999998</v>
+        <v>2.27</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B73">
         <v>2.2599999999999998</v>
@@ -1401,7 +1404,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B74">
         <v>2.2599999999999998</v>
@@ -1409,15 +1412,15 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B75">
-        <v>2.25</v>
+        <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B76">
         <v>2.25</v>
@@ -1425,15 +1428,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>60</v>
       </c>
       <c r="B77">
-        <v>2.2400000000000002</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="B78">
         <v>2.2400000000000002</v>
@@ -1441,15 +1444,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B79">
-        <v>2.23</v>
+        <v>2.2400000000000002</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B80">
         <v>2.23</v>
@@ -1457,7 +1460,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>143</v>
       </c>
       <c r="B81">
         <v>2.23</v>
@@ -1465,7 +1468,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B82">
         <v>2.23</v>
@@ -1473,7 +1476,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
       <c r="B83">
         <v>2.23</v>
@@ -1481,7 +1484,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>72</v>
+        <v>136</v>
       </c>
       <c r="B84">
         <v>2.23</v>
@@ -1489,15 +1492,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B85">
-        <v>2.2200000000000002</v>
+        <v>2.23</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B86">
         <v>2.2200000000000002</v>
@@ -1505,7 +1508,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B87">
         <v>2.2200000000000002</v>
@@ -1513,15 +1516,15 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B88">
-        <v>2.21</v>
+        <v>2.2200000000000002</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B89">
         <v>2.21</v>
@@ -1529,15 +1532,15 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>138</v>
+        <v>71</v>
       </c>
       <c r="B90">
-        <v>2.2000000000000002</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="B91">
         <v>2.2000000000000002</v>
@@ -1545,7 +1548,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>151</v>
+        <v>72</v>
       </c>
       <c r="B92">
         <v>2.2000000000000002</v>
@@ -1553,15 +1556,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>80</v>
+        <v>141</v>
       </c>
       <c r="B93">
-        <v>2.19</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B94">
         <v>2.19</v>
@@ -1569,15 +1572,15 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B95">
-        <v>2.1800000000000002</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B96">
         <v>2.1800000000000002</v>
@@ -1585,7 +1588,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B97">
         <v>2.1800000000000002</v>
@@ -1593,15 +1596,15 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="B98">
-        <v>2.17</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>149</v>
+        <v>78</v>
       </c>
       <c r="B99">
         <v>2.17</v>
@@ -1609,39 +1612,39 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>86</v>
+        <v>139</v>
       </c>
       <c r="B100">
-        <v>2.16</v>
+        <v>2.17</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B101">
-        <v>2.15</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B102">
-        <v>2.14</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B103">
-        <v>2.13</v>
+        <v>2.14</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B104">
         <v>2.13</v>
@@ -1649,7 +1652,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B105">
         <v>2.13</v>
@@ -1657,7 +1660,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="B106">
         <v>2.13</v>
@@ -1665,7 +1668,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B107">
         <v>2.13</v>
@@ -1673,15 +1676,15 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B108">
-        <v>2.12</v>
+        <v>2.13</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B109">
         <v>2.12</v>
@@ -1689,31 +1692,31 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B110">
-        <v>2.11</v>
+        <v>2.12</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B111">
-        <v>2.1</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="B112">
-        <v>2.09</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B113">
         <v>2.09</v>
@@ -1721,15 +1724,15 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B114">
-        <v>2.08</v>
+        <v>2.09</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B115">
         <v>2.08</v>
@@ -1737,15 +1740,15 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B116">
-        <v>2.0699999999999998</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B117">
         <v>2.0699999999999998</v>
@@ -1753,7 +1756,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B118">
         <v>2.0699999999999998</v>
@@ -1761,23 +1764,23 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B119">
-        <v>2.06</v>
+        <v>2.0699999999999998</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>147</v>
+        <v>95</v>
       </c>
       <c r="B120">
-        <v>2.0499999999999998</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="B121">
         <v>2.0499999999999998</v>
@@ -1785,15 +1788,15 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>107</v>
+        <v>138</v>
       </c>
       <c r="B122">
-        <v>2.0299999999999998</v>
+        <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B123">
         <v>2.0299999999999998</v>
@@ -1801,15 +1804,15 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B124">
-        <v>2.02</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B125">
         <v>2.02</v>
@@ -1817,15 +1820,15 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B126">
-        <v>2.0099999999999998</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B127">
         <v>2.0099999999999998</v>
@@ -1833,7 +1836,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B128">
         <v>2.0099999999999998</v>
@@ -1841,23 +1844,23 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B129">
-        <v>2</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
       <c r="B130">
-        <v>1.99</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B131">
         <v>1.99</v>
@@ -1865,7 +1868,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B132">
         <v>1.99</v>
@@ -1873,23 +1876,23 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B133">
-        <v>1.98</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B134">
-        <v>1.97</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="B135">
         <v>1.97</v>
@@ -1897,15 +1900,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B136">
-        <v>1.94</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B137">
         <v>1.94</v>
@@ -1913,15 +1916,15 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B138">
-        <v>1.91</v>
+        <v>1.94</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B139">
         <v>1.91</v>
@@ -1929,15 +1932,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B140">
-        <v>1.89</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B141">
         <v>1.89</v>
@@ -1945,71 +1948,71 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="B142">
-        <v>1.86</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="B143">
-        <v>1.85</v>
+        <v>1.86</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B144">
-        <v>1.82</v>
+        <v>1.85</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B145">
-        <v>1.78</v>
+        <v>1.82</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B146">
-        <v>1.74</v>
+        <v>1.78</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B147">
-        <v>1.73</v>
+        <v>1.74</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B148">
-        <v>1.68</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B149">
-        <v>1.67</v>
+        <v>1.68</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B150">
         <v>1.67</v>
@@ -2017,17 +2020,25 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B151">
-        <v>1.57</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="B152">
+        <v>1.57</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>126</v>
+      </c>
+      <c r="B153">
         <v>1.43</v>
       </c>
     </row>

</xml_diff>